<commit_message>
changed my github username and email
</commit_message>
<xml_diff>
--- a/CS335/GitHub Info sans duplicates.xlsx
+++ b/CS335/GitHub Info sans duplicates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\xampp\htdocs\lungo\staffcard\CS335\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\staffcard-master\CS335\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72B3928A-6D71-435A-A1C9-9542474283ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4752A6A9-A448-4985-BB14-583626C8C1F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1125" yWindow="1125" windowWidth="15375" windowHeight="8325" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3331" uniqueCount="931">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3331" uniqueCount="932">
   <si>
     <t>Timestamp</t>
   </si>
@@ -2820,6 +2820,9 @@
   </si>
   <si>
     <t>https://github.com/Sikato-41</t>
+  </si>
+  <si>
+    <t>NDIO</t>
   </si>
 </sst>
 </file>
@@ -3327,9 +3330,9 @@
   <dimension ref="A1:X137"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A118" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A103" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="E134" sqref="E134"/>
+      <selection pane="bottomLeft" activeCell="F107" sqref="F107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7339,7 +7342,7 @@
         <v>749</v>
       </c>
       <c r="F106" s="3" t="s">
-        <v>16</v>
+        <v>931</v>
       </c>
       <c r="H106" s="3" t="s">
         <v>27</v>

</xml_diff>